<commit_message>
add FeatureConfiguration for LWB and MWB
</commit_message>
<xml_diff>
--- a/docs/LanguageWorkbench_FeatureConfiguration.xlsx
+++ b/docs/LanguageWorkbench_FeatureConfiguration.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28429"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20417"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\tgiraudet\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="Z:\git\github\gemoc\ql-gemoc-lwb2025\docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0BAAF3E9-8E5C-4999-A5BE-3E0F27BB1FE4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FC002B70-8F05-43E3-B5D3-8789284A153B}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{7FD4AA70-ECA5-4D89-879B-07B2E8F8F0C4}"/>
   </bookViews>
@@ -20,22 +20,12 @@
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:Single"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
-        <xcalcf:feature name="microsoft.com:CNMTM"/>
-        <xcalcf:feature name="microsoft.com:LET_WF"/>
-        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
-      </xcalcf:calcFeatures>
-    </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="244" uniqueCount="153">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="369" uniqueCount="169">
   <si>
     <t>Language Workbench</t>
   </si>
@@ -43,9 +33,6 @@
     <t>Feature</t>
   </si>
   <si>
-    <t>&lt;Language workbench name&gt;</t>
-  </si>
-  <si>
     <t>Comments</t>
   </si>
   <si>
@@ -494,6 +481,57 @@
   </si>
   <si>
     <t>│   └── Versioning</t>
+  </si>
+  <si>
+    <t>for textual, graphical and tree concrete syntaxes</t>
+  </si>
+  <si>
+    <t>Supported by the graphical editor (Sirius); Unsure about capabilities of Xtext on this, not supported by the EMF tree editor</t>
+  </si>
+  <si>
+    <t>Supported by the graphical editor (Sirius); Supported by the textual editor (Xtext), not supported by the EMF tree editor</t>
+  </si>
+  <si>
+    <t>Supported by the graphical editor (Sirius), but unsure about capabiltes of Xtext on this; not supported by the EMF tree editor</t>
+  </si>
+  <si>
+    <t>Supported by the EMF tree editor only</t>
+  </si>
+  <si>
+    <t>Graphical editor uses a .design file to define the mapping; Xtext uses a .xtext file to define the grammar</t>
+  </si>
+  <si>
+    <t>with GEMOC Sequential Engine</t>
+  </si>
+  <si>
+    <t>With GEMOC Concurrent Engine and use of MOCML</t>
+  </si>
+  <si>
+    <t>For both Graphical and textual syntaxes</t>
+  </si>
+  <si>
+    <t>For both Graphical (autolayout) and textual syntaxes</t>
+  </si>
+  <si>
+    <t>For all syntaxes (Graphical, textual and tree), support of Eclipse IDE to customize almost anything</t>
+  </si>
+  <si>
+    <t>For textual syntax only, not relevant for graphical syntaxes</t>
+  </si>
+  <si>
+    <t>With EMF diff for graphical, and IDE for textual</t>
+  </si>
+  <si>
+    <t>Fully supported for Graphical Editor; not supported for textual editor</t>
+  </si>
+  <si>
+    <t>Depend on the editor used to edit the metamodel</t>
+  </si>
+  <si>
+    <t>Depend on the editor used to edit the metamodel, (textual using OCLInEcore editor, tree or graphical)</t>
+  </si>
+  <si>
+    <t>GEMOC Studio</t>
   </si>
 </sst>
 </file>
@@ -624,9 +662,6 @@
   </cellStyles>
   <dxfs count="2">
     <dxf>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
       <font>
         <strike val="0"/>
         <outline val="0"/>
@@ -640,6 +675,9 @@
         <scheme val="none"/>
       </font>
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -655,11 +693,11 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{386018CC-2DD9-414B-A04F-9CCD124002F8}" name="Tableau2" displayName="Tableau2" ref="A1:C145" totalsRowShown="0" headerRowDxfId="0">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{386018CC-2DD9-414B-A04F-9CCD124002F8}" name="Tableau2" displayName="Tableau2" ref="A1:C145" totalsRowShown="0" headerRowDxfId="1">
   <autoFilter ref="A1:C145" xr:uid="{386018CC-2DD9-414B-A04F-9CCD124002F8}"/>
   <tableColumns count="3">
-    <tableColumn id="1" xr3:uid="{B406174F-A27E-4E0E-91B4-F2C68E845F5A}" name="Feature" dataDxfId="1"/>
-    <tableColumn id="2" xr3:uid="{30F54B26-B672-4A8D-BBBF-87E3312A1E8C}" name="&lt;Language workbench name&gt;"/>
+    <tableColumn id="1" xr3:uid="{B406174F-A27E-4E0E-91B4-F2C68E845F5A}" name="Feature" dataDxfId="0"/>
+    <tableColumn id="2" xr3:uid="{30F54B26-B672-4A8D-BBBF-87E3312A1E8C}" name="GEMOC Studio"/>
     <tableColumn id="3" xr3:uid="{DE361FCB-B5CF-4524-8295-676BC12229C6}" name="Comments"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium3" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
@@ -966,1045 +1004,1420 @@
   <dimension ref="A1:F145"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E22" sqref="E22"/>
+      <selection activeCell="E3" sqref="E3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="54.453125" customWidth="1"/>
-    <col min="2" max="2" width="31.453125" customWidth="1"/>
+    <col min="1" max="1" width="54.42578125" customWidth="1"/>
+    <col min="2" max="2" width="31.42578125" customWidth="1"/>
     <col min="3" max="3" width="21" customWidth="1"/>
     <col min="5" max="5" width="16" customWidth="1"/>
-    <col min="6" max="6" width="47.36328125" customWidth="1"/>
+    <col min="6" max="6" width="47.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" s="7" t="s">
         <v>1</v>
       </c>
       <c r="B1" s="7" t="s">
+        <v>168</v>
+      </c>
+      <c r="C1" s="7" t="s">
         <v>2</v>
       </c>
-      <c r="C1" s="7" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.35">
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" s="8" t="s">
         <v>0</v>
       </c>
       <c r="B2" s="7" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C2" s="7" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.35">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" s="8" t="s">
+        <v>9</v>
+      </c>
+      <c r="B3" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="C3" s="7" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A4" s="8" t="s">
         <v>10</v>
       </c>
-      <c r="B3" s="7" t="s">
-        <v>8</v>
-      </c>
-      <c r="C3" s="7" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A4" s="8" t="s">
+      <c r="B4" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="C4" s="7" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A5" s="8" t="s">
         <v>11</v>
       </c>
-      <c r="B4" s="7" t="s">
-        <v>8</v>
-      </c>
-      <c r="C4" s="7" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A5" s="8" t="s">
+      <c r="B5" s="3" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A6" s="8" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="6" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A6" s="8" t="s">
+      <c r="B6" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="C6" s="7" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A7" s="8" t="s">
         <v>13</v>
       </c>
-      <c r="B6" s="7" t="s">
-        <v>8</v>
-      </c>
-      <c r="C6" s="7" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A7" s="8" t="s">
+      <c r="B7" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="C7" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="E7" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="F7" s="2"/>
+    </row>
+    <row r="8" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A8" s="8" t="s">
         <v>14</v>
       </c>
-      <c r="B7" s="7" t="s">
-        <v>8</v>
-      </c>
-      <c r="C7" s="7" t="s">
-        <v>8</v>
-      </c>
-      <c r="E7" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="F7" s="2"/>
-    </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A8" s="8" t="s">
-        <v>15</v>
+      <c r="B8" s="5" t="s">
+        <v>6</v>
       </c>
       <c r="E8" s="3"/>
       <c r="F8" s="4"/>
     </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A9" s="8" t="s">
+        <v>15</v>
+      </c>
+      <c r="B9" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="E9" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="F9" s="4"/>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A10" s="8" t="s">
         <v>16</v>
       </c>
-      <c r="E9" s="3" t="s">
+      <c r="B10" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="C10" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="E10" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="F9" s="4"/>
-    </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A10" s="8" t="s">
+      <c r="F10" s="4" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A11" s="8" t="s">
         <v>17</v>
       </c>
-      <c r="B10" s="7" t="s">
-        <v>8</v>
-      </c>
-      <c r="C10" s="7" t="s">
-        <v>8</v>
-      </c>
-      <c r="E10" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="F10" s="4" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="11" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A11" s="8" t="s">
+      <c r="B11" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="E11" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="F11" s="6"/>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A12" s="8" t="s">
         <v>18</v>
       </c>
-      <c r="E11" s="5" t="s">
-        <v>7</v>
-      </c>
-      <c r="F11" s="6"/>
-    </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A12" s="8" t="s">
+      <c r="B12" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="C12" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A13" s="8" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A13" s="8" t="s">
+      <c r="B13" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="C13" s="7" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A14" s="8" t="s">
         <v>20</v>
       </c>
-      <c r="B13" s="7" t="s">
-        <v>8</v>
-      </c>
-      <c r="C13" s="7" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A14" s="8" t="s">
+      <c r="B14" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="C14" s="7" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A15" s="8" t="s">
         <v>21</v>
       </c>
-      <c r="B14" s="7" t="s">
-        <v>8</v>
-      </c>
-      <c r="C14" s="7" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A15" s="8" t="s">
+      <c r="B15" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="C15" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A16" s="8" t="s">
         <v>22</v>
       </c>
-    </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A16" s="8" t="s">
+      <c r="B16" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="C16" t="s">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A17" s="8" t="s">
         <v>23</v>
       </c>
-    </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A17" s="8" t="s">
+      <c r="B17" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="C17" t="s">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A18" s="8" t="s">
         <v>24</v>
       </c>
-    </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A18" s="8" t="s">
+      <c r="B18" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="C18" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A19" s="8" t="s">
         <v>25</v>
       </c>
-    </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A19" s="8" t="s">
+      <c r="B19" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="C19" s="7" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A20" s="8" t="s">
         <v>26</v>
       </c>
-      <c r="B19" s="7" t="s">
-        <v>8</v>
-      </c>
-      <c r="C19" s="7" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A20" s="8" t="s">
+      <c r="B20" s="3"/>
+      <c r="C20" t="s">
+        <v>156</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A21" s="8" t="s">
         <v>27</v>
       </c>
-    </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A21" s="8" t="s">
+      <c r="B21" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="C21" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A22" s="8" t="s">
         <v>28</v>
       </c>
-    </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A22" s="8" t="s">
+      <c r="B22" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="C22" s="7" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A23" s="8" t="s">
         <v>29</v>
       </c>
-      <c r="B22" s="7" t="s">
-        <v>8</v>
-      </c>
-      <c r="C22" s="7" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A23" s="8" t="s">
+      <c r="B23" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="C23" s="7" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A24" s="8" t="s">
         <v>30</v>
       </c>
-      <c r="B23" s="7" t="s">
-        <v>8</v>
-      </c>
-      <c r="C23" s="7" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A24" s="8" t="s">
+      <c r="B24" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="C24" s="7" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A25" s="8" t="s">
         <v>31</v>
       </c>
-      <c r="B24" s="7" t="s">
-        <v>8</v>
-      </c>
-      <c r="C24" s="7" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A25" s="8" t="s">
+      <c r="B25" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="C25" s="7" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A26" s="8" t="s">
         <v>32</v>
       </c>
-      <c r="B25" s="7" t="s">
-        <v>8</v>
-      </c>
-      <c r="C25" s="7" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="26" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A26" s="8" t="s">
+      <c r="B26" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="C26" s="7" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="27" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A27" s="8" t="s">
         <v>33</v>
       </c>
-      <c r="B26" s="7" t="s">
-        <v>8</v>
-      </c>
-      <c r="C26" s="7" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="27" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A27" s="8" t="s">
+      <c r="B27" s="3" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="28" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A28" s="8" t="s">
         <v>34</v>
       </c>
-    </row>
-    <row r="28" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A28" s="8" t="s">
+      <c r="B28" s="3" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="29" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A29" s="8" t="s">
         <v>35</v>
       </c>
-    </row>
-    <row r="29" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A29" s="8" t="s">
+      <c r="B29" s="3" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="30" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A30" s="8" t="s">
         <v>36</v>
       </c>
-    </row>
-    <row r="30" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A30" s="8" t="s">
+      <c r="B30" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="C30" s="7"/>
+    </row>
+    <row r="31" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A31" s="8" t="s">
         <v>37</v>
       </c>
-      <c r="B30" s="7"/>
-      <c r="C30" s="7"/>
-    </row>
-    <row r="31" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A31" s="8" t="s">
+      <c r="B31" s="3" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="32" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A32" s="8" t="s">
         <v>38</v>
       </c>
-    </row>
-    <row r="32" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A32" s="8" t="s">
+      <c r="B32" s="3" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="33" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A33" s="8" t="s">
         <v>39</v>
       </c>
-    </row>
-    <row r="33" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A33" s="8" t="s">
+      <c r="B33" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="C33" s="7" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="34" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A34" s="8" t="s">
         <v>40</v>
       </c>
-      <c r="B33" s="7" t="s">
-        <v>8</v>
-      </c>
-      <c r="C33" s="7" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="34" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A34" s="8" t="s">
+      <c r="B34" s="3" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="35" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A35" s="8" t="s">
         <v>41</v>
       </c>
-    </row>
-    <row r="35" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A35" s="8" t="s">
+      <c r="B35" s="3" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="36" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A36" s="8" t="s">
         <v>42</v>
       </c>
-    </row>
-    <row r="36" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A36" s="8" t="s">
+      <c r="B36" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="C36" s="7" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="37" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A37" s="8" t="s">
         <v>43</v>
       </c>
-      <c r="B36" s="7" t="s">
-        <v>8</v>
-      </c>
-      <c r="C36" s="7" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="37" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A37" s="8" t="s">
+      <c r="B37" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="C37" t="s">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="38" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A38" s="8" t="s">
         <v>44</v>
       </c>
-    </row>
-    <row r="38" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A38" s="8" t="s">
+      <c r="B38" s="5" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="39" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A39" s="8" t="s">
         <v>45</v>
       </c>
-    </row>
-    <row r="39" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A39" s="8" t="s">
+      <c r="B39" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="C39" t="s">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="40" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A40" s="8" t="s">
         <v>46</v>
       </c>
-    </row>
-    <row r="40" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A40" s="8" t="s">
+      <c r="B40" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="C40" s="7" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="41" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A41" s="8" t="s">
         <v>47</v>
       </c>
-      <c r="B40" s="7" t="s">
-        <v>8</v>
-      </c>
-      <c r="C40" s="7" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="41" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A41" s="8" t="s">
+      <c r="B41" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="C41" s="7" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="42" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A42" s="8" t="s">
         <v>48</v>
       </c>
-      <c r="B41" s="7" t="s">
-        <v>8</v>
-      </c>
-      <c r="C41" s="7" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="42" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A42" s="8" t="s">
+      <c r="B42" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="C42" t="s">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="43" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A43" s="8" t="s">
         <v>49</v>
       </c>
-    </row>
-    <row r="43" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A43" s="8" t="s">
+      <c r="B43" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="C43" t="s">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="44" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A44" s="8" t="s">
         <v>50</v>
       </c>
-    </row>
-    <row r="44" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A44" s="8" t="s">
+      <c r="B44" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="C44" t="s">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="45" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A45" s="8" t="s">
         <v>51</v>
       </c>
-    </row>
-    <row r="45" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A45" s="8" t="s">
+      <c r="B45" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="C45" t="s">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="46" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A46" s="8" t="s">
         <v>52</v>
       </c>
-    </row>
-    <row r="46" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A46" s="8" t="s">
+      <c r="B46" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="C46" s="7" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="47" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A47" s="8" t="s">
         <v>53</v>
       </c>
-      <c r="B46" s="7" t="s">
-        <v>8</v>
-      </c>
-      <c r="C46" s="7" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="47" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A47" s="8" t="s">
+      <c r="B47" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="C47" t="s">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="48" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A48" s="8" t="s">
         <v>54</v>
       </c>
-    </row>
-    <row r="48" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A48" s="8" t="s">
+      <c r="B48" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="C48" t="s">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="49" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A49" s="8" t="s">
         <v>55</v>
       </c>
-    </row>
-    <row r="49" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A49" s="8" t="s">
+      <c r="B49" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="C49" s="7" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="50" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A50" s="8" t="s">
         <v>56</v>
       </c>
-      <c r="B49" s="7" t="s">
-        <v>8</v>
-      </c>
-      <c r="C49" s="7" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="50" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A50" s="8" t="s">
+      <c r="B50" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="C50" t="s">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="51" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A51" s="8" t="s">
         <v>57</v>
       </c>
-    </row>
-    <row r="51" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A51" s="8" t="s">
+      <c r="B51" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="C51" s="7" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="52" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A52" s="8" t="s">
         <v>58</v>
       </c>
-      <c r="B51" s="7" t="s">
-        <v>8</v>
-      </c>
-      <c r="C51" s="7" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="52" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A52" s="8" t="s">
+      <c r="B52" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="C52" t="s">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="53" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A53" s="8" t="s">
         <v>59</v>
       </c>
-    </row>
-    <row r="53" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A53" s="8" t="s">
+      <c r="B53" s="5" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="54" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A54" s="8" t="s">
         <v>60</v>
       </c>
-    </row>
-    <row r="54" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A54" s="8" t="s">
+      <c r="B54" s="3" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="55" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A55" s="8" t="s">
         <v>61</v>
       </c>
-    </row>
-    <row r="55" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A55" s="8" t="s">
+      <c r="B55" s="5" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="56" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A56" s="8" t="s">
         <v>62</v>
       </c>
-    </row>
-    <row r="56" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A56" s="8" t="s">
+      <c r="B56" s="5" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="57" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A57" s="8" t="s">
         <v>63</v>
       </c>
-    </row>
-    <row r="57" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A57" s="8" t="s">
+      <c r="B57" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="C57" t="s">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="58" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A58" s="8" t="s">
         <v>64</v>
       </c>
-    </row>
-    <row r="58" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A58" s="8" t="s">
+      <c r="B58" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="C58" s="7" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="59" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A59" s="8" t="s">
         <v>65</v>
       </c>
-      <c r="B58" s="7" t="s">
-        <v>8</v>
-      </c>
-      <c r="C58" s="7" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="59" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A59" s="8" t="s">
+      <c r="B59" s="3" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="60" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A60" s="8" t="s">
         <v>66</v>
       </c>
-    </row>
-    <row r="60" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A60" s="8" t="s">
+      <c r="B60" s="3" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="61" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A61" s="8" t="s">
         <v>67</v>
       </c>
-    </row>
-    <row r="61" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A61" s="8" t="s">
+      <c r="B61" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="C61" s="7" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="62" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A62" s="8" t="s">
         <v>68</v>
       </c>
-      <c r="B61" s="7" t="s">
-        <v>8</v>
-      </c>
-      <c r="C61" s="7" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="62" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A62" s="8" t="s">
+      <c r="B62" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="C62" s="7" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="63" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A63" s="8" t="s">
         <v>69</v>
       </c>
-      <c r="B62" s="7" t="s">
-        <v>8</v>
-      </c>
-      <c r="C62" s="7" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="63" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A63" s="8" t="s">
+      <c r="B63" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="C63" t="s">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="64" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A64" s="8" t="s">
         <v>70</v>
       </c>
-    </row>
-    <row r="64" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A64" s="8" t="s">
+      <c r="B64" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="C64" t="s">
+        <v>166</v>
+      </c>
+    </row>
+    <row r="65" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A65" s="8" t="s">
         <v>71</v>
       </c>
-    </row>
-    <row r="65" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A65" s="8" t="s">
+      <c r="B65" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="C65" t="s">
+        <v>166</v>
+      </c>
+    </row>
+    <row r="66" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A66" s="8" t="s">
         <v>72</v>
       </c>
-    </row>
-    <row r="66" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A66" s="8" t="s">
+      <c r="B66" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="C66" s="7" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="67" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A67" s="8" t="s">
         <v>73</v>
       </c>
-      <c r="B66" s="7" t="s">
-        <v>8</v>
-      </c>
-      <c r="C66" s="7" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="67" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A67" s="8" t="s">
+      <c r="B67" s="3" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="68" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A68" s="8" t="s">
         <v>74</v>
       </c>
-    </row>
-    <row r="68" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A68" s="8" t="s">
+      <c r="B68" s="3" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="69" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A69" s="8" t="s">
         <v>75</v>
       </c>
-    </row>
-    <row r="69" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A69" s="8" t="s">
+      <c r="B69" s="3" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="70" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A70" s="8" t="s">
         <v>76</v>
       </c>
-    </row>
-    <row r="70" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A70" s="8" t="s">
+      <c r="B70" s="3" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="71" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A71" s="8" t="s">
         <v>77</v>
       </c>
-    </row>
-    <row r="71" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A71" s="8" t="s">
+      <c r="B71" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="C71" t="s">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="72" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A72" s="8" t="s">
         <v>78</v>
       </c>
-    </row>
-    <row r="72" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A72" s="8" t="s">
+      <c r="B72" s="3" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="73" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A73" s="8" t="s">
         <v>79</v>
       </c>
-    </row>
-    <row r="73" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A73" s="8" t="s">
+      <c r="B73" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="C73" s="7" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="74" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A74" s="8" t="s">
         <v>80</v>
       </c>
-      <c r="B73" s="7" t="s">
-        <v>8</v>
-      </c>
-      <c r="C73" s="7" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="74" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A74" s="8" t="s">
+      <c r="B74" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="C74" t="s">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="75" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A75" s="8" t="s">
         <v>81</v>
       </c>
-    </row>
-    <row r="75" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A75" s="8" t="s">
+      <c r="B75" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="C75" t="s">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="76" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A76" s="8" t="s">
         <v>82</v>
       </c>
-    </row>
-    <row r="76" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A76" s="8" t="s">
+      <c r="B76" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="C76" t="s">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="77" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A77" s="8" t="s">
         <v>83</v>
       </c>
-    </row>
-    <row r="77" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A77" s="8" t="s">
+      <c r="B77" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="C77" t="s">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="78" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A78" s="8" t="s">
         <v>84</v>
       </c>
-    </row>
-    <row r="78" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A78" s="8" t="s">
+      <c r="B78" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="C78" t="s">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="79" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A79" s="8" t="s">
         <v>85</v>
       </c>
     </row>
-    <row r="79" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A79" s="8" t="s">
+    <row r="80" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A80" s="8" t="s">
         <v>86</v>
       </c>
-    </row>
-    <row r="80" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A80" s="8" t="s">
+      <c r="B80" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="C80" t="s">
+        <v>165</v>
+      </c>
+    </row>
+    <row r="81" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A81" s="8" t="s">
         <v>87</v>
       </c>
-    </row>
-    <row r="81" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A81" s="8" t="s">
+      <c r="B81" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="C81" s="7" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="82" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A82" s="8" t="s">
         <v>88</v>
       </c>
-      <c r="B81" s="7" t="s">
-        <v>8</v>
-      </c>
-      <c r="C81" s="7" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="82" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A82" s="8" t="s">
+      <c r="B82" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="C82" t="s">
+        <v>165</v>
+      </c>
+    </row>
+    <row r="83" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A83" s="8" t="s">
         <v>89</v>
       </c>
-    </row>
-    <row r="83" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A83" s="8" t="s">
+      <c r="B83" s="3" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="84" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A84" s="8" t="s">
         <v>90</v>
       </c>
-    </row>
-    <row r="84" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A84" s="8" t="s">
+      <c r="B84" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="C84" s="7" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="85" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A85" s="8" t="s">
         <v>91</v>
       </c>
-      <c r="B84" s="7" t="s">
-        <v>8</v>
-      </c>
-      <c r="C84" s="7" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="85" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A85" s="8" t="s">
+      <c r="B85" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="C85" s="7" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="86" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A86" s="8" t="s">
         <v>92</v>
       </c>
-      <c r="B85" s="7" t="s">
-        <v>8</v>
-      </c>
-      <c r="C85" s="7" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="86" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A86" s="8" t="s">
+      <c r="B86" s="3" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="87" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A87" s="8" t="s">
         <v>93</v>
       </c>
-    </row>
-    <row r="87" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A87" s="8" t="s">
+      <c r="B87" s="5" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="88" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A88" s="8" t="s">
         <v>94</v>
       </c>
-    </row>
-    <row r="88" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A88" s="8" t="s">
+      <c r="B88" s="3" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="89" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A89" s="8" t="s">
         <v>95</v>
       </c>
-    </row>
-    <row r="89" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A89" s="8" t="s">
+      <c r="B89" s="5" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="90" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A90" s="8" t="s">
         <v>96</v>
       </c>
-    </row>
-    <row r="90" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A90" s="8" t="s">
+      <c r="B90" s="3" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="91" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A91" s="8" t="s">
         <v>97</v>
       </c>
-    </row>
-    <row r="91" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A91" s="8" t="s">
+      <c r="B91" s="5" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="92" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A92" s="8" t="s">
         <v>98</v>
       </c>
-    </row>
-    <row r="92" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A92" s="8" t="s">
+      <c r="B92" s="5" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="93" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A93" s="8" t="s">
         <v>99</v>
       </c>
-    </row>
-    <row r="93" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A93" s="8" t="s">
+      <c r="B93" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="C93" s="7" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="94" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A94" s="8" t="s">
         <v>100</v>
       </c>
-      <c r="B93" s="7" t="s">
-        <v>8</v>
-      </c>
-      <c r="C93" s="7" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="94" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A94" s="8" t="s">
+      <c r="B94" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="C94" s="7" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="95" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A95" s="8" t="s">
         <v>101</v>
       </c>
-      <c r="B94" s="7" t="s">
-        <v>8</v>
-      </c>
-      <c r="C94" s="7" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="95" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A95" s="8" t="s">
+      <c r="B95" s="5" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="96" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A96" s="8" t="s">
         <v>102</v>
       </c>
-    </row>
-    <row r="96" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A96" s="8" t="s">
+      <c r="B96" s="5" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="97" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A97" s="8" t="s">
         <v>103</v>
       </c>
-    </row>
-    <row r="97" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A97" s="8" t="s">
+      <c r="B97" s="5" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="98" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A98" s="8" t="s">
         <v>104</v>
       </c>
-    </row>
-    <row r="98" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A98" s="8" t="s">
+      <c r="B98" s="5" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="99" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A99" s="8" t="s">
         <v>105</v>
       </c>
-    </row>
-    <row r="99" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A99" s="8" t="s">
+      <c r="B99" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="C99" s="7" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="100" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A100" s="8" t="s">
         <v>106</v>
       </c>
-      <c r="B99" s="7" t="s">
-        <v>8</v>
-      </c>
-      <c r="C99" s="7" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="100" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A100" s="8" t="s">
+      <c r="B100" s="5" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="101" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A101" s="8" t="s">
         <v>107</v>
       </c>
-    </row>
-    <row r="101" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A101" s="8" t="s">
+      <c r="B101" s="3" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="102" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A102" s="8" t="s">
         <v>108</v>
       </c>
-    </row>
-    <row r="102" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A102" s="8" t="s">
+      <c r="B102" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="C102" s="7" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="103" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A103" s="8" t="s">
         <v>109</v>
       </c>
-      <c r="B102" s="7" t="s">
-        <v>8</v>
-      </c>
-      <c r="C102" s="7" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="103" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A103" s="8" t="s">
+      <c r="B103" s="3" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="104" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A104" s="8" t="s">
         <v>110</v>
       </c>
-    </row>
-    <row r="104" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A104" s="8" t="s">
+      <c r="B104" s="5" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="105" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A105" s="8" t="s">
         <v>111</v>
       </c>
-    </row>
-    <row r="105" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A105" s="8" t="s">
+      <c r="B105" s="5" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="106" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A106" s="8" t="s">
         <v>112</v>
       </c>
-    </row>
-    <row r="106" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A106" s="8" t="s">
+      <c r="B106" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="C106" s="7" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="107" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A107" s="8" t="s">
         <v>113</v>
       </c>
-      <c r="B106" s="7" t="s">
-        <v>8</v>
-      </c>
-      <c r="C106" s="7" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="107" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A107" s="8" t="s">
+      <c r="B107" s="3" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="108" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A108" s="8" t="s">
         <v>114</v>
       </c>
-    </row>
-    <row r="108" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A108" s="8" t="s">
+      <c r="B108" s="3" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="109" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A109" s="8" t="s">
         <v>115</v>
       </c>
-    </row>
-    <row r="109" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A109" s="8" t="s">
+      <c r="B109" s="3" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="110" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A110" s="8" t="s">
         <v>116</v>
       </c>
-    </row>
-    <row r="110" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A110" s="8" t="s">
+      <c r="B110" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="C110" s="7" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="111" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A111" s="8" t="s">
         <v>117</v>
       </c>
-      <c r="B110" s="7" t="s">
-        <v>8</v>
-      </c>
-      <c r="C110" s="7" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="111" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A111" s="8" t="s">
+      <c r="B111" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="C111" s="7" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="112" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A112" s="8" t="s">
         <v>118</v>
       </c>
-      <c r="B111" s="7" t="s">
-        <v>8</v>
-      </c>
-      <c r="C111" s="7" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="112" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A112" s="8" t="s">
+      <c r="B112" s="3" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="113" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A113" s="8" t="s">
         <v>119</v>
       </c>
-    </row>
-    <row r="113" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A113" s="8" t="s">
+      <c r="B113" s="3" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="114" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A114" s="8" t="s">
         <v>120</v>
       </c>
-    </row>
-    <row r="114" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A114" s="8" t="s">
+      <c r="B114" s="3" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="115" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A115" s="8" t="s">
         <v>121</v>
       </c>
-    </row>
-    <row r="115" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A115" s="8" t="s">
+      <c r="B115" s="3" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="116" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A116" s="8" t="s">
         <v>122</v>
       </c>
-    </row>
-    <row r="116" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A116" s="8" t="s">
+      <c r="B116" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="C116" s="7" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="117" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A117" s="8" t="s">
         <v>123</v>
       </c>
-      <c r="B116" s="7" t="s">
-        <v>8</v>
-      </c>
-      <c r="C116" s="7" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="117" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A117" s="8" t="s">
+      <c r="B117" s="3" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="118" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A118" s="8" t="s">
         <v>124</v>
       </c>
-    </row>
-    <row r="118" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A118" s="8" t="s">
+      <c r="B118" s="3" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="119" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A119" s="8" t="s">
         <v>125</v>
       </c>
-    </row>
-    <row r="119" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A119" s="8" t="s">
+      <c r="B119" s="3" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="120" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A120" s="8" t="s">
         <v>126</v>
       </c>
-    </row>
-    <row r="120" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A120" s="8" t="s">
+      <c r="B120" s="3" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="121" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A121" s="8" t="s">
         <v>127</v>
       </c>
-    </row>
-    <row r="121" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A121" s="8" t="s">
+      <c r="B121" s="5" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="122" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A122" s="8" t="s">
         <v>128</v>
       </c>
-    </row>
-    <row r="122" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A122" s="8" t="s">
+      <c r="B122" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="C122" s="7" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="123" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A123" s="8" t="s">
         <v>129</v>
       </c>
-      <c r="B122" s="7" t="s">
-        <v>8</v>
-      </c>
-      <c r="C122" s="7" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="123" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A123" s="8" t="s">
+      <c r="B123" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="C123" s="7" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="124" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A124" s="8" t="s">
         <v>130</v>
       </c>
-      <c r="B123" s="7" t="s">
-        <v>8</v>
-      </c>
-      <c r="C123" s="7" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="124" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A124" s="8" t="s">
+      <c r="B124" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="C124" s="7" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="125" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A125" s="8" t="s">
         <v>131</v>
       </c>
-      <c r="B124" s="7" t="s">
-        <v>8</v>
-      </c>
-      <c r="C124" s="7" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="125" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A125" s="8" t="s">
+      <c r="B125" s="3" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="126" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A126" s="8" t="s">
         <v>132</v>
       </c>
-    </row>
-    <row r="126" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A126" s="8" t="s">
+      <c r="B126" s="5" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="127" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A127" s="8" t="s">
         <v>133</v>
       </c>
-    </row>
-    <row r="127" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A127" s="8" t="s">
+      <c r="B127" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="C127" s="7" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="128" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A128" s="8" t="s">
         <v>134</v>
       </c>
-      <c r="B127" s="7" t="s">
-        <v>8</v>
-      </c>
-      <c r="C127" s="7" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="128" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A128" s="8" t="s">
+      <c r="B128" s="3" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="129" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A129" s="8" t="s">
         <v>135</v>
       </c>
-    </row>
-    <row r="129" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A129" s="8" t="s">
+      <c r="B129" s="3" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="130" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A130" s="8" t="s">
+        <v>151</v>
+      </c>
+      <c r="B130" s="3" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="131" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A131" s="8" t="s">
         <v>136</v>
       </c>
-    </row>
-    <row r="130" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A130" s="8" t="s">
-        <v>152</v>
-      </c>
-    </row>
-    <row r="131" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A131" s="8" t="s">
+      <c r="B131" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="C131" s="7" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="132" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A132" s="8" t="s">
         <v>137</v>
       </c>
-      <c r="B131" s="7" t="s">
-        <v>8</v>
-      </c>
-      <c r="C131" s="7" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="132" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A132" s="8" t="s">
+      <c r="B132" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="C132" s="7" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="133" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A133" s="8" t="s">
         <v>138</v>
       </c>
-      <c r="B132" s="7" t="s">
-        <v>8</v>
-      </c>
-      <c r="C132" s="7" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="133" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A133" s="8" t="s">
+      <c r="B133" s="3" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="134" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A134" s="8" t="s">
         <v>139</v>
       </c>
-    </row>
-    <row r="134" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A134" s="8" t="s">
+      <c r="B134" s="5" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="135" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A135" s="8" t="s">
+        <v>149</v>
+      </c>
+      <c r="B135" s="3" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="136" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A136" s="8" t="s">
         <v>140</v>
       </c>
-    </row>
-    <row r="135" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A135" s="8" t="s">
+      <c r="B136" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="C136" s="7" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="137" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A137" s="8" t="s">
+        <v>141</v>
+      </c>
+      <c r="B137" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="C137" s="7" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="138" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A138" s="8" t="s">
+        <v>142</v>
+      </c>
+      <c r="B138" s="3" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="139" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A139" s="8" t="s">
+        <v>143</v>
+      </c>
+      <c r="B139" s="5" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="140" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A140" s="8" t="s">
         <v>150</v>
       </c>
-    </row>
-    <row r="136" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A136" s="8" t="s">
-        <v>141</v>
-      </c>
-      <c r="B136" s="7" t="s">
-        <v>8</v>
-      </c>
-      <c r="C136" s="7" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="137" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A137" s="8" t="s">
-        <v>142</v>
-      </c>
-      <c r="B137" s="7" t="s">
-        <v>8</v>
-      </c>
-      <c r="C137" s="7" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="138" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A138" s="8" t="s">
-        <v>143</v>
-      </c>
-    </row>
-    <row r="139" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A139" s="8" t="s">
+      <c r="B140" s="5" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="141" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A141" s="8" t="s">
         <v>144</v>
       </c>
-    </row>
-    <row r="140" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A140" s="8" t="s">
-        <v>151</v>
-      </c>
-    </row>
-    <row r="141" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A141" s="8" t="s">
+      <c r="B141" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="C141" s="7" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="142" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A142" s="8" t="s">
         <v>145</v>
       </c>
-      <c r="B141" s="7" t="s">
-        <v>8</v>
-      </c>
-      <c r="C141" s="7" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="142" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A142" s="8" t="s">
+      <c r="B142" s="5" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="143" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A143" s="8" t="s">
         <v>146</v>
       </c>
-    </row>
-    <row r="143" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A143" s="8" t="s">
+      <c r="B143" s="5" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="144" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A144" s="8" t="s">
         <v>147</v>
       </c>
-    </row>
-    <row r="144" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A144" s="8" t="s">
+      <c r="B144" s="5" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="145" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A145" s="8" t="s">
         <v>148</v>
       </c>
-    </row>
-    <row r="145" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A145" s="8" t="s">
-        <v>149</v>
+      <c r="B145" s="5" t="s">
+        <v>6</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
updated feature table documents with QLS
</commit_message>
<xml_diff>
--- a/docs/LanguageWorkbench_FeatureConfiguration.xlsx
+++ b/docs/LanguageWorkbench_FeatureConfiguration.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="Z:\git\github\gemoc\ql-gemoc-lwb2025\docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FC002B70-8F05-43E3-B5D3-8789284A153B}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{285E4271-02FB-4754-82C6-A86306533B32}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{7FD4AA70-ECA5-4D89-879B-07B2E8F8F0C4}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="369" uniqueCount="169">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="370" uniqueCount="170">
   <si>
     <t>Language Workbench</t>
   </si>
@@ -532,6 +532,9 @@
   </si>
   <si>
     <t>GEMOC Studio</t>
+  </si>
+  <si>
+    <t>Provide wizards and documentation</t>
   </si>
 </sst>
 </file>
@@ -1004,7 +1007,7 @@
   <dimension ref="A1:F145"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E3" sqref="E3"/>
+      <selection activeCell="C6" sqref="C6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1065,7 +1068,10 @@
         <v>11</v>
       </c>
       <c r="B5" s="3" t="s">
-        <v>4</v>
+        <v>5</v>
+      </c>
+      <c r="C5" t="s">
+        <v>169</v>
       </c>
     </row>
     <row r="6" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">

</xml_diff>

<commit_message>
take into account some remarks
</commit_message>
<xml_diff>
--- a/docs/LanguageWorkbench_FeatureConfiguration.xlsx
+++ b/docs/LanguageWorkbench_FeatureConfiguration.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="Z:\git\github\gemoc\ql-gemoc-lwb2025\docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{285E4271-02FB-4754-82C6-A86306533B32}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E60BFDD2-2B03-4E3C-9519-02D99A614BCC}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{7FD4AA70-ECA5-4D89-879B-07B2E8F8F0C4}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="370" uniqueCount="170">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="372" uniqueCount="171">
   <si>
     <t>Language Workbench</t>
   </si>
@@ -535,6 +535,9 @@
   </si>
   <si>
     <t>Provide wizards and documentation</t>
+  </si>
+  <si>
+    <t>depend on the used metalanguage (sequential or concurrent)</t>
   </si>
 </sst>
 </file>
@@ -1006,8 +1009,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A0467C85-CDFA-45E8-AEAF-B61FBEF68F92}">
   <dimension ref="A1:F145"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C6" sqref="C6"/>
+    <sheetView tabSelected="1" topLeftCell="A85" workbookViewId="0">
+      <selection activeCell="C107" sqref="C107"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1574,12 +1577,12 @@
         <v>160</v>
       </c>
     </row>
-    <row r="53" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="53" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A53" s="8" t="s">
         <v>59</v>
       </c>
-      <c r="B53" s="5" t="s">
-        <v>6</v>
+      <c r="B53" s="3" t="s">
+        <v>4</v>
       </c>
     </row>
     <row r="54" spans="1:3" x14ac:dyDescent="0.25">
@@ -1919,12 +1922,12 @@
         <v>4</v>
       </c>
     </row>
-    <row r="89" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="89" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A89" s="8" t="s">
         <v>95</v>
       </c>
-      <c r="B89" s="5" t="s">
-        <v>6</v>
+      <c r="B89" s="3" t="s">
+        <v>4</v>
       </c>
     </row>
     <row r="90" spans="1:3" x14ac:dyDescent="0.25">
@@ -1997,12 +2000,12 @@
         <v>6</v>
       </c>
     </row>
-    <row r="98" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="98" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A98" s="8" t="s">
         <v>104</v>
       </c>
-      <c r="B98" s="5" t="s">
-        <v>6</v>
+      <c r="B98" s="3" t="s">
+        <v>4</v>
       </c>
     </row>
     <row r="99" spans="1:3" x14ac:dyDescent="0.25">
@@ -2016,12 +2019,15 @@
         <v>7</v>
       </c>
     </row>
-    <row r="100" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="100" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A100" s="8" t="s">
         <v>106</v>
       </c>
-      <c r="B100" s="5" t="s">
-        <v>6</v>
+      <c r="B100" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="C100" t="s">
+        <v>170</v>
       </c>
     </row>
     <row r="101" spans="1:3" x14ac:dyDescent="0.25">
@@ -2030,6 +2036,9 @@
       </c>
       <c r="B101" s="3" t="s">
         <v>4</v>
+      </c>
+      <c r="C101" t="s">
+        <v>170</v>
       </c>
     </row>
     <row r="102" spans="1:3" x14ac:dyDescent="0.25">

</xml_diff>